<commit_message>
add new conditions to check_list
</commit_message>
<xml_diff>
--- a/Form_testing_(Check_list).xlsx
+++ b/Form_testing_(Check_list).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880"/>
   </bookViews>
   <sheets>
     <sheet name="Требования к форме" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="409">
   <si>
     <t>Поле "Name:"</t>
   </si>
@@ -1283,6 +1283,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Привести placeholder-текст к единому образцу</t>
+  </si>
+  <si>
+    <t>отсекать пробелы в конце/начале пароля</t>
+  </si>
+  <si>
+    <t>глазик для пароля</t>
+  </si>
+  <si>
+    <t>подсказка для поля пароля какие можно вводить символы</t>
+  </si>
+  <si>
+    <t>добавить номер тел при регистрации</t>
   </si>
 </sst>
 </file>
@@ -1514,6 +1526,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1553,32 +1577,20 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3074,55 +3086,55 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A2:M32"/>
+  <dimension ref="A2:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
     </row>
     <row r="4" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26" t="s">
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -3184,14 +3196,14 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" ref="A10" si="0">1+A9</f>
+        <f>1+A9</f>
         <v>3</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10" si="1">1+H9</f>
+        <f>1+H9</f>
         <v>3</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -3204,18 +3216,18 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" ref="A11:A16" si="2">1+A10</f>
+        <f>1+A10</f>
         <v>4</v>
       </c>
       <c r="B11" t="s">
         <v>68</v>
       </c>
       <c r="H11">
-        <f t="shared" ref="H11:H16" si="3">1+H10</f>
+        <f>1+H10</f>
         <v>4</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>2</v>
+      <c r="I11" t="s">
+        <v>68</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -3224,14 +3236,14 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="2"/>
+        <f>1+A11</f>
         <v>5</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H12">
-        <f t="shared" si="3"/>
+        <f>1+H11</f>
         <v>5</v>
       </c>
       <c r="I12" s="5" t="s">
@@ -3244,18 +3256,18 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="2"/>
+        <f>1+A12</f>
         <v>6</v>
       </c>
-      <c r="B13" t="s">
-        <v>17</v>
+      <c r="B13" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="H13">
-        <f t="shared" si="3"/>
+        <f>1+H12</f>
         <v>6</v>
       </c>
-      <c r="I13" t="s">
-        <v>17</v>
+      <c r="I13" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -3264,18 +3276,18 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="2"/>
+        <f>1+A13</f>
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H14">
-        <f t="shared" si="3"/>
+        <f>1+H13</f>
         <v>7</v>
       </c>
       <c r="I14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -3284,18 +3296,18 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="2"/>
+        <f>1+A14</f>
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H15">
-        <f t="shared" si="3"/>
+        <f>1+H14</f>
         <v>8</v>
       </c>
       <c r="I15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -3304,18 +3316,18 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="2"/>
+        <f>1+A15</f>
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="H16">
-        <f t="shared" si="3"/>
+        <f>1+H15</f>
         <v>9</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>5</v>
+      <c r="I16" t="s">
+        <v>19</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -3323,243 +3335,256 @@
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="3"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="I18" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>1</v>
       </c>
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="B19" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="3"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19" t="s">
-        <v>27</v>
-      </c>
+      <c r="I19" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="9"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f>1+A19</f>
         <v>2</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
       <c r="H20">
-        <f>1+H19</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" ref="A21:A32" si="4">1+A20</f>
+        <f t="shared" ref="A21:A32" si="0">1+A20</f>
         <v>3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+        <v>26</v>
+      </c>
       <c r="H21">
-        <f t="shared" ref="H21:H24" si="5">1+H20</f>
-        <v>3</v>
+        <f>1+H20</f>
+        <v>2</v>
       </c>
       <c r="I21" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
       <c r="H22">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" ref="H22:H25" si="1">1+H21</f>
+        <v>3</v>
       </c>
       <c r="I22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="H23">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="I23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
       <c r="H24">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="I24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H25">
-        <f>1+H24</f>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="I25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>29</v>
+      <c r="B26" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="H26">
         <f>1+H25</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I26" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
       <c r="H27">
         <f>1+H26</f>
-        <v>9</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="I27" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="H28">
+        <f>1+H27</f>
+        <v>9</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>178</v>
+      <c r="B29" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>6</v>
+        <v>176</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3582,8 +3607,8 @@
   </sheetPr>
   <dimension ref="A1:Z38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3598,26 +3623,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -3683,7 +3708,7 @@
       <c r="D5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="35" t="s">
         <v>55</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -3708,7 +3733,7 @@
       <c r="D6" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="36"/>
       <c r="F6" s="8" t="s">
         <v>38</v>
       </c>
@@ -3728,7 +3753,7 @@
       <c r="D7" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E7" s="33"/>
+      <c r="E7" s="37"/>
       <c r="F7" s="8" t="s">
         <v>38</v>
       </c>
@@ -3748,7 +3773,7 @@
       <c r="D8" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="38" t="s">
         <v>47</v>
       </c>
       <c r="F8" s="15" t="s">
@@ -3772,7 +3797,7 @@
       <c r="D9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="35"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="8" t="s">
         <v>39</v>
       </c>
@@ -3794,7 +3819,7 @@
       <c r="D10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="35"/>
+      <c r="E10" s="39"/>
       <c r="F10" s="8" t="s">
         <v>39</v>
       </c>
@@ -3816,7 +3841,7 @@
       <c r="D11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="36"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="8" t="s">
         <v>39</v>
       </c>
@@ -3858,7 +3883,7 @@
       <c r="D13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="38" t="s">
         <v>47</v>
       </c>
       <c r="F13" s="8" t="s">
@@ -3880,7 +3905,7 @@
       <c r="D14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="35"/>
+      <c r="E14" s="39"/>
       <c r="F14" s="8" t="s">
         <v>38</v>
       </c>
@@ -3900,7 +3925,7 @@
       <c r="D15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="36"/>
+      <c r="E15" s="40"/>
       <c r="F15" s="8" t="s">
         <v>39</v>
       </c>
@@ -3944,7 +3969,7 @@
       <c r="D17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="38" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="8" t="s">
@@ -3968,7 +3993,7 @@
       <c r="D18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="36"/>
+      <c r="E18" s="40"/>
       <c r="F18" s="8" t="s">
         <v>39</v>
       </c>
@@ -3990,7 +4015,7 @@
       <c r="D19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="38" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="8" t="s">
@@ -4012,7 +4037,7 @@
       <c r="D20" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E20" s="35"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="8" t="s">
         <v>38</v>
       </c>
@@ -4032,7 +4057,7 @@
       <c r="D21" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E21" s="35"/>
+      <c r="E21" s="39"/>
       <c r="F21" s="8" t="s">
         <v>38</v>
       </c>
@@ -4052,7 +4077,7 @@
       <c r="D22" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E22" s="35"/>
+      <c r="E22" s="39"/>
       <c r="F22" s="8" t="s">
         <v>38</v>
       </c>
@@ -4072,7 +4097,7 @@
       <c r="D23" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="35"/>
+      <c r="E23" s="39"/>
       <c r="F23" s="8" t="s">
         <v>38</v>
       </c>
@@ -4092,7 +4117,7 @@
       <c r="D24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="36"/>
+      <c r="E24" s="40"/>
       <c r="F24" s="8" t="s">
         <v>38</v>
       </c>
@@ -4158,7 +4183,7 @@
       <c r="D27" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="38" t="s">
         <v>55</v>
       </c>
       <c r="F27" s="8" t="s">
@@ -4182,7 +4207,7 @@
       <c r="D28" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="35"/>
+      <c r="E28" s="39"/>
       <c r="F28" s="8" t="s">
         <v>39</v>
       </c>
@@ -4204,7 +4229,7 @@
       <c r="D29" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="35"/>
+      <c r="E29" s="39"/>
       <c r="F29" s="8" t="s">
         <v>39</v>
       </c>
@@ -4226,7 +4251,7 @@
       <c r="D30" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="36"/>
+      <c r="E30" s="40"/>
       <c r="F30" s="8" t="s">
         <v>39</v>
       </c>
@@ -4248,7 +4273,7 @@
       <c r="D31" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="38" t="s">
         <v>47</v>
       </c>
       <c r="F31" s="8" t="s">
@@ -4270,7 +4295,7 @@
       <c r="D32" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="36"/>
+      <c r="E32" s="40"/>
       <c r="F32" s="8" t="s">
         <v>39</v>
       </c>
@@ -4459,26 +4484,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4544,7 +4569,7 @@
       <c r="D5" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="35" t="s">
         <v>55</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -4569,7 +4594,7 @@
       <c r="D6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="36"/>
       <c r="F6" s="8" t="s">
         <v>38</v>
       </c>
@@ -4589,7 +4614,7 @@
       <c r="D7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="33"/>
+      <c r="E7" s="37"/>
       <c r="F7" s="8" t="s">
         <v>38</v>
       </c>
@@ -4609,7 +4634,7 @@
       <c r="D8" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="38" t="s">
         <v>47</v>
       </c>
       <c r="F8" s="15" t="s">
@@ -4633,7 +4658,7 @@
       <c r="D9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="35"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="8" t="s">
         <v>39</v>
       </c>
@@ -4655,7 +4680,7 @@
       <c r="D10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="35"/>
+      <c r="E10" s="39"/>
       <c r="F10" s="8" t="s">
         <v>39</v>
       </c>
@@ -4677,7 +4702,7 @@
       <c r="D11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="36"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="8" t="s">
         <v>39</v>
       </c>
@@ -4719,7 +4744,7 @@
       <c r="D13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="38" t="s">
         <v>47</v>
       </c>
       <c r="F13" s="8" t="s">
@@ -4741,7 +4766,7 @@
       <c r="D14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="35"/>
+      <c r="E14" s="39"/>
       <c r="F14" s="8" t="s">
         <v>38</v>
       </c>
@@ -4761,7 +4786,7 @@
       <c r="D15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="36"/>
+      <c r="E15" s="40"/>
       <c r="F15" s="8" t="s">
         <v>39</v>
       </c>
@@ -4805,7 +4830,7 @@
       <c r="D17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="38" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="8" t="s">
@@ -4829,7 +4854,7 @@
       <c r="D18" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E18" s="36"/>
+      <c r="E18" s="40"/>
       <c r="F18" s="8" t="s">
         <v>39</v>
       </c>
@@ -4851,7 +4876,7 @@
       <c r="D19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="38" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="8" t="s">
@@ -4873,7 +4898,7 @@
       <c r="D20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="35"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="8" t="s">
         <v>38</v>
       </c>
@@ -4893,7 +4918,7 @@
       <c r="D21" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="35"/>
+      <c r="E21" s="39"/>
       <c r="F21" s="8" t="s">
         <v>38</v>
       </c>
@@ -4913,7 +4938,7 @@
       <c r="D22" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="35"/>
+      <c r="E22" s="39"/>
       <c r="F22" s="8" t="s">
         <v>38</v>
       </c>
@@ -4933,7 +4958,7 @@
       <c r="D23" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E23" s="35"/>
+      <c r="E23" s="39"/>
       <c r="F23" s="8" t="s">
         <v>38</v>
       </c>
@@ -4953,7 +4978,7 @@
       <c r="D24" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E24" s="36"/>
+      <c r="E24" s="40"/>
       <c r="F24" s="8" t="s">
         <v>38</v>
       </c>
@@ -5019,7 +5044,7 @@
       <c r="D27" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="38" t="s">
         <v>55</v>
       </c>
       <c r="F27" s="8" t="s">
@@ -5041,7 +5066,7 @@
       <c r="D28" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E28" s="35"/>
+      <c r="E28" s="39"/>
       <c r="F28" s="8" t="s">
         <v>38</v>
       </c>
@@ -5061,7 +5086,7 @@
       <c r="D29" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E29" s="35"/>
+      <c r="E29" s="39"/>
       <c r="F29" s="8" t="s">
         <v>38</v>
       </c>
@@ -5081,7 +5106,7 @@
       <c r="D30" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="36"/>
+      <c r="E30" s="40"/>
       <c r="F30" s="8" t="s">
         <v>38</v>
       </c>
@@ -5101,7 +5126,7 @@
       <c r="D31" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="38" t="s">
         <v>47</v>
       </c>
       <c r="F31" s="8" t="s">
@@ -5125,7 +5150,7 @@
       <c r="D32" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="36"/>
+      <c r="E32" s="40"/>
       <c r="F32" s="8" t="s">
         <v>39</v>
       </c>
@@ -5292,7 +5317,7 @@
   </sheetPr>
   <dimension ref="A1:Z71"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -5308,26 +5333,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -5391,7 +5416,7 @@
       <c r="D5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="35" t="s">
         <v>55</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -5416,7 +5441,7 @@
       <c r="D6" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="36"/>
       <c r="F6" s="8" t="s">
         <v>38</v>
       </c>
@@ -5436,7 +5461,7 @@
       <c r="D7" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="36"/>
       <c r="F7" s="8" t="s">
         <v>38</v>
       </c>
@@ -5456,7 +5481,7 @@
       <c r="D8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="33"/>
+      <c r="E8" s="37"/>
       <c r="F8" s="8" t="s">
         <v>38</v>
       </c>
@@ -5476,7 +5501,7 @@
       <c r="D9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="38" t="s">
         <v>47</v>
       </c>
       <c r="F9" s="8" t="s">
@@ -5500,7 +5525,7 @@
       <c r="D10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="35"/>
+      <c r="E10" s="39"/>
       <c r="F10" s="8" t="s">
         <v>39</v>
       </c>
@@ -5522,7 +5547,7 @@
       <c r="D11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="35"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="8" t="s">
         <v>39</v>
       </c>
@@ -5544,7 +5569,7 @@
       <c r="D12" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="8" t="s">
         <v>39</v>
       </c>
@@ -5566,7 +5591,7 @@
       <c r="D13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="35"/>
+      <c r="E13" s="39"/>
       <c r="F13" s="8" t="s">
         <v>39</v>
       </c>
@@ -5588,7 +5613,7 @@
       <c r="D14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="35"/>
+      <c r="E14" s="39"/>
       <c r="F14" s="8" t="s">
         <v>39</v>
       </c>
@@ -5610,7 +5635,7 @@
       <c r="D15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="35"/>
+      <c r="E15" s="39"/>
       <c r="F15" s="8" t="s">
         <v>39</v>
       </c>
@@ -5632,7 +5657,7 @@
       <c r="D16" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E16" s="35"/>
+      <c r="E16" s="39"/>
       <c r="F16" s="8" t="s">
         <v>39</v>
       </c>
@@ -5654,7 +5679,7 @@
       <c r="D17" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E17" s="35"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="8" t="s">
         <v>39</v>
       </c>
@@ -5676,7 +5701,7 @@
       <c r="D18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="35"/>
+      <c r="E18" s="39"/>
       <c r="F18" s="8" t="s">
         <v>39</v>
       </c>
@@ -5698,7 +5723,7 @@
       <c r="D19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="35"/>
+      <c r="E19" s="39"/>
       <c r="F19" s="8" t="s">
         <v>39</v>
       </c>
@@ -5720,7 +5745,7 @@
       <c r="D20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="36"/>
+      <c r="E20" s="40"/>
       <c r="F20" s="8" t="s">
         <v>39</v>
       </c>
@@ -5742,7 +5767,7 @@
       <c r="D21" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="35" t="s">
         <v>55</v>
       </c>
       <c r="F21" s="8" t="s">
@@ -5764,7 +5789,7 @@
       <c r="D22" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="32"/>
+      <c r="E22" s="36"/>
       <c r="F22" s="15" t="s">
         <v>38</v>
       </c>
@@ -5784,7 +5809,7 @@
       <c r="D23" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="32"/>
+      <c r="E23" s="36"/>
       <c r="F23" s="8" t="s">
         <v>38</v>
       </c>
@@ -5804,7 +5829,7 @@
       <c r="D24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="33"/>
+      <c r="E24" s="37"/>
       <c r="F24" s="8" t="s">
         <v>38</v>
       </c>
@@ -5824,7 +5849,7 @@
       <c r="D25" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="E25" s="38" t="s">
         <v>47</v>
       </c>
       <c r="F25" s="8" t="s">
@@ -5848,7 +5873,7 @@
       <c r="D26" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="35"/>
+      <c r="E26" s="39"/>
       <c r="F26" s="8" t="s">
         <v>39</v>
       </c>
@@ -5870,7 +5895,7 @@
       <c r="D27" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="35"/>
+      <c r="E27" s="39"/>
       <c r="F27" s="8" t="s">
         <v>39</v>
       </c>
@@ -5892,7 +5917,7 @@
       <c r="D28" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="35"/>
+      <c r="E28" s="39"/>
       <c r="F28" s="8" t="s">
         <v>39</v>
       </c>
@@ -5914,7 +5939,7 @@
       <c r="D29" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="36"/>
+      <c r="E29" s="40"/>
       <c r="F29" s="8" t="s">
         <v>39</v>
       </c>
@@ -5958,7 +5983,7 @@
       <c r="D31" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="38" t="s">
         <v>47</v>
       </c>
       <c r="F31" s="8" t="s">
@@ -5982,7 +6007,7 @@
       <c r="D32" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="35"/>
+      <c r="E32" s="39"/>
       <c r="F32" s="8" t="s">
         <v>39</v>
       </c>
@@ -6004,7 +6029,7 @@
       <c r="D33" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="35"/>
+      <c r="E33" s="39"/>
       <c r="F33" s="8" t="s">
         <v>39</v>
       </c>
@@ -6026,7 +6051,7 @@
       <c r="D34" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E34" s="36"/>
+      <c r="E34" s="40"/>
       <c r="F34" s="8" t="s">
         <v>39</v>
       </c>
@@ -6094,7 +6119,7 @@
       <c r="D37" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E37" s="34" t="s">
+      <c r="E37" s="38" t="s">
         <v>55</v>
       </c>
       <c r="F37" s="8" t="s">
@@ -6116,7 +6141,7 @@
       <c r="D38" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E38" s="35"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="8" t="s">
         <v>38</v>
       </c>
@@ -6136,7 +6161,7 @@
       <c r="D39" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="36"/>
+      <c r="E39" s="40"/>
       <c r="F39" s="8" t="s">
         <v>38</v>
       </c>
@@ -6156,7 +6181,7 @@
       <c r="D40" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E40" s="34" t="s">
+      <c r="E40" s="38" t="s">
         <v>47</v>
       </c>
       <c r="F40" s="8" t="s">
@@ -6180,7 +6205,7 @@
       <c r="D41" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E41" s="35"/>
+      <c r="E41" s="39"/>
       <c r="F41" s="8" t="s">
         <v>39</v>
       </c>
@@ -6202,7 +6227,7 @@
       <c r="D42" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E42" s="35"/>
+      <c r="E42" s="39"/>
       <c r="F42" s="8" t="s">
         <v>39</v>
       </c>
@@ -6224,7 +6249,7 @@
       <c r="D43" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E43" s="35"/>
+      <c r="E43" s="39"/>
       <c r="F43" s="8" t="s">
         <v>39</v>
       </c>
@@ -6246,7 +6271,7 @@
       <c r="D44" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E44" s="35"/>
+      <c r="E44" s="39"/>
       <c r="F44" s="8" t="s">
         <v>39</v>
       </c>
@@ -6268,7 +6293,7 @@
       <c r="D45" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E45" s="35"/>
+      <c r="E45" s="39"/>
       <c r="F45" s="8" t="s">
         <v>39</v>
       </c>
@@ -6290,7 +6315,7 @@
       <c r="D46" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E46" s="35"/>
+      <c r="E46" s="39"/>
       <c r="F46" s="8" t="s">
         <v>39</v>
       </c>
@@ -6312,7 +6337,7 @@
       <c r="D47" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E47" s="35"/>
+      <c r="E47" s="39"/>
       <c r="F47" s="8" t="s">
         <v>39</v>
       </c>
@@ -6334,7 +6359,7 @@
       <c r="D48" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E48" s="35"/>
+      <c r="E48" s="39"/>
       <c r="F48" s="8" t="s">
         <v>39</v>
       </c>
@@ -6356,7 +6381,7 @@
       <c r="D49" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E49" s="35"/>
+      <c r="E49" s="39"/>
       <c r="F49" s="8" t="s">
         <v>39</v>
       </c>
@@ -6378,7 +6403,7 @@
       <c r="D50" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E50" s="36"/>
+      <c r="E50" s="40"/>
       <c r="F50" s="16" t="s">
         <v>39</v>
       </c>
@@ -6823,7 +6848,7 @@
   </sheetPr>
   <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -6839,26 +6864,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -6971,7 +6996,7 @@
       <c r="D7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="38" t="s">
         <v>47</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -6995,7 +7020,7 @@
       <c r="D8" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E8" s="35"/>
+      <c r="E8" s="39"/>
       <c r="F8" s="8" t="s">
         <v>39</v>
       </c>
@@ -7017,7 +7042,7 @@
       <c r="D9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="35"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="8" t="s">
         <v>39</v>
       </c>
@@ -7039,7 +7064,7 @@
       <c r="D10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="35"/>
+      <c r="E10" s="39"/>
       <c r="F10" s="8" t="s">
         <v>39</v>
       </c>
@@ -7061,7 +7086,7 @@
       <c r="D11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="35"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="8" t="s">
         <v>39</v>
       </c>
@@ -7151,7 +7176,7 @@
       <c r="D15" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="35" t="s">
         <v>47</v>
       </c>
       <c r="F15" s="8" t="s">
@@ -7175,7 +7200,7 @@
       <c r="D16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="32"/>
+      <c r="E16" s="36"/>
       <c r="F16" s="8" t="s">
         <v>39</v>
       </c>
@@ -7197,7 +7222,7 @@
       <c r="D17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="32"/>
+      <c r="E17" s="36"/>
       <c r="F17" s="8" t="s">
         <v>39</v>
       </c>
@@ -7219,7 +7244,7 @@
       <c r="D18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="32"/>
+      <c r="E18" s="36"/>
       <c r="F18" s="8" t="s">
         <v>39</v>
       </c>
@@ -7241,7 +7266,7 @@
       <c r="D19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="32"/>
+      <c r="E19" s="36"/>
       <c r="F19" s="8" t="s">
         <v>39</v>
       </c>
@@ -7263,7 +7288,7 @@
       <c r="D20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="32"/>
+      <c r="E20" s="36"/>
       <c r="F20" s="8" t="s">
         <v>39</v>
       </c>
@@ -7285,7 +7310,7 @@
       <c r="D21" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="32"/>
+      <c r="E21" s="36"/>
       <c r="F21" s="8" t="s">
         <v>39</v>
       </c>
@@ -7307,7 +7332,7 @@
       <c r="D22" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="33"/>
+      <c r="E22" s="37"/>
       <c r="F22" s="8" t="s">
         <v>39</v>
       </c>
@@ -7351,7 +7376,7 @@
       <c r="D24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="35" t="s">
         <v>47</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -7375,7 +7400,7 @@
       <c r="D25" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="33"/>
+      <c r="E25" s="37"/>
       <c r="F25" s="8" t="s">
         <v>39</v>
       </c>
@@ -7397,7 +7422,7 @@
       <c r="D26" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="31" t="s">
+      <c r="E26" s="35" t="s">
         <v>55</v>
       </c>
       <c r="F26" s="8" t="s">
@@ -7419,7 +7444,7 @@
       <c r="D27" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E27" s="32"/>
+      <c r="E27" s="36"/>
       <c r="F27" s="8" t="s">
         <v>38</v>
       </c>
@@ -7439,7 +7464,7 @@
       <c r="D28" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="33"/>
+      <c r="E28" s="37"/>
       <c r="F28" s="8" t="s">
         <v>38</v>
       </c>
@@ -7459,7 +7484,7 @@
       <c r="D29" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="35" t="s">
         <v>47</v>
       </c>
       <c r="F29" s="8" t="s">
@@ -7483,7 +7508,7 @@
       <c r="D30" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="33"/>
+      <c r="E30" s="37"/>
       <c r="F30" s="18" t="s">
         <v>39</v>
       </c>
@@ -7944,7 +7969,7 @@
   </sheetPr>
   <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -7960,26 +7985,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -8070,7 +8095,7 @@
       <c r="D6" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="41" t="s">
         <v>47</v>
       </c>
       <c r="F6" s="8" t="s">
@@ -8092,7 +8117,7 @@
       <c r="D7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="39"/>
+      <c r="E7" s="42"/>
       <c r="F7" s="8" t="s">
         <v>39</v>
       </c>
@@ -8114,7 +8139,7 @@
       <c r="D8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="38"/>
+      <c r="E8" s="43"/>
       <c r="F8" s="8" t="s">
         <v>39</v>
       </c>
@@ -8243,7 +8268,7 @@
       <c r="D14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="26" t="s">
         <v>376</v>
       </c>
       <c r="F14" s="8" t="s">
@@ -8285,7 +8310,7 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
-      <c r="C18" s="40"/>
+      <c r="C18" s="25"/>
       <c r="D18" s="17"/>
       <c r="E18"/>
       <c r="F18" s="17"/>
@@ -8852,250 +8877,265 @@
   <dimension ref="A2:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" style="42" customWidth="1"/>
+    <col min="1" max="1" width="8" style="27" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>394</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26" t="s">
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
     </row>
     <row r="7" spans="2:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
     </row>
     <row r="8" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>1</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="44" t="s">
         <v>395</v>
       </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
     </row>
     <row r="9" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>2</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="44" t="s">
         <v>396</v>
       </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
     </row>
     <row r="10" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>3</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="44" t="s">
         <v>397</v>
       </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
     </row>
     <row r="11" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>4</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="45" t="s">
         <v>398</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
     </row>
     <row r="12" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>5</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="44" t="s">
         <v>404</v>
       </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
     </row>
     <row r="13" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>6</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="44" t="s">
         <v>399</v>
       </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
     </row>
     <row r="14" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>7</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="44" t="s">
         <v>400</v>
       </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
     </row>
     <row r="15" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>8</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="45" t="s">
         <v>401</v>
       </c>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="46"/>
-      <c r="K15" s="46"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
     </row>
     <row r="16" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>9</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="44" t="s">
         <v>402</v>
       </c>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
     </row>
     <row r="17" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
         <v>10</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="44" t="s">
         <v>403</v>
       </c>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
+      <c r="C18" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
+      <c r="C19" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
+      <c r="C20" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
+      <c r="A21" s="28"/>
+      <c r="C21" t="s">
+        <v>408</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
+      <c r="A27" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:K3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:K4"/>
     <mergeCell ref="C14:K14"/>
     <mergeCell ref="C15:K15"/>
     <mergeCell ref="C16:K16"/>
@@ -9107,9 +9147,6 @@
     <mergeCell ref="C11:K11"/>
     <mergeCell ref="C12:K12"/>
     <mergeCell ref="C13:K13"/>
-    <mergeCell ref="B2:K3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:K4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" display="http://itcareer.pythonanywhere.com/"/>

</xml_diff>

<commit_message>
translate few sheets inside check_list
</commit_message>
<xml_diff>
--- a/Form_testing_(Check_list).xlsx
+++ b/Form_testing_(Check_list).xlsx
@@ -12,12 +12,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="Требования к форме" sheetId="1" r:id="rId1"/>
+    <sheet name="Form requirements" sheetId="1" r:id="rId1"/>
     <sheet name="Name" sheetId="2" r:id="rId2"/>
     <sheet name="Surname" sheetId="6" r:id="rId3"/>
     <sheet name="Email" sheetId="7" r:id="rId4"/>
     <sheet name="Password" sheetId="9" r:id="rId5"/>
-    <sheet name="Все поля" sheetId="10" r:id="rId6"/>
+    <sheet name="All fields" sheetId="10" r:id="rId6"/>
     <sheet name="Improvements" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -1578,6 +1578,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1623,18 +1626,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1643,6 +1634,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3141,52 +3141,52 @@
   <dimension ref="A2:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
     </row>
     <row r="4" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -3675,26 +3675,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
     </row>
     <row r="3" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -3760,7 +3760,7 @@
       <c r="D5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="36" t="s">
         <v>55</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -3785,7 +3785,7 @@
       <c r="D6" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E6" s="36"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="8" t="s">
         <v>38</v>
       </c>
@@ -3805,7 +3805,7 @@
       <c r="D7" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E7" s="37"/>
+      <c r="E7" s="38"/>
       <c r="F7" s="8" t="s">
         <v>38</v>
       </c>
@@ -3825,7 +3825,7 @@
       <c r="D8" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="39" t="s">
         <v>47</v>
       </c>
       <c r="F8" s="15" t="s">
@@ -3849,7 +3849,7 @@
       <c r="D9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="39"/>
+      <c r="E9" s="40"/>
       <c r="F9" s="8" t="s">
         <v>39</v>
       </c>
@@ -3871,7 +3871,7 @@
       <c r="D10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="39"/>
+      <c r="E10" s="40"/>
       <c r="F10" s="8" t="s">
         <v>39</v>
       </c>
@@ -3893,7 +3893,7 @@
       <c r="D11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="40"/>
+      <c r="E11" s="41"/>
       <c r="F11" s="8" t="s">
         <v>39</v>
       </c>
@@ -3935,7 +3935,7 @@
       <c r="D13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="39" t="s">
         <v>47</v>
       </c>
       <c r="F13" s="8" t="s">
@@ -3957,7 +3957,7 @@
       <c r="D14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="39"/>
+      <c r="E14" s="40"/>
       <c r="F14" s="8" t="s">
         <v>38</v>
       </c>
@@ -3977,7 +3977,7 @@
       <c r="D15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="40"/>
+      <c r="E15" s="41"/>
       <c r="F15" s="8" t="s">
         <v>39</v>
       </c>
@@ -4021,7 +4021,7 @@
       <c r="D17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="39" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="8" t="s">
@@ -4045,7 +4045,7 @@
       <c r="D18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="40"/>
+      <c r="E18" s="41"/>
       <c r="F18" s="8" t="s">
         <v>39</v>
       </c>
@@ -4067,7 +4067,7 @@
       <c r="D19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="39" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="8" t="s">
@@ -4089,7 +4089,7 @@
       <c r="D20" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E20" s="39"/>
+      <c r="E20" s="40"/>
       <c r="F20" s="8" t="s">
         <v>38</v>
       </c>
@@ -4109,7 +4109,7 @@
       <c r="D21" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E21" s="39"/>
+      <c r="E21" s="40"/>
       <c r="F21" s="8" t="s">
         <v>38</v>
       </c>
@@ -4129,7 +4129,7 @@
       <c r="D22" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E22" s="39"/>
+      <c r="E22" s="40"/>
       <c r="F22" s="8" t="s">
         <v>38</v>
       </c>
@@ -4149,7 +4149,7 @@
       <c r="D23" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="39"/>
+      <c r="E23" s="40"/>
       <c r="F23" s="8" t="s">
         <v>38</v>
       </c>
@@ -4169,7 +4169,7 @@
       <c r="D24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="40"/>
+      <c r="E24" s="41"/>
       <c r="F24" s="8" t="s">
         <v>38</v>
       </c>
@@ -4235,7 +4235,7 @@
       <c r="D27" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="39" t="s">
         <v>55</v>
       </c>
       <c r="F27" s="8" t="s">
@@ -4259,7 +4259,7 @@
       <c r="D28" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="39"/>
+      <c r="E28" s="40"/>
       <c r="F28" s="8" t="s">
         <v>39</v>
       </c>
@@ -4281,7 +4281,7 @@
       <c r="D29" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="39"/>
+      <c r="E29" s="40"/>
       <c r="F29" s="8" t="s">
         <v>39</v>
       </c>
@@ -4303,7 +4303,7 @@
       <c r="D30" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="40"/>
+      <c r="E30" s="41"/>
       <c r="F30" s="8" t="s">
         <v>39</v>
       </c>
@@ -4325,7 +4325,7 @@
       <c r="D31" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="38" t="s">
+      <c r="E31" s="39" t="s">
         <v>47</v>
       </c>
       <c r="F31" s="8" t="s">
@@ -4347,7 +4347,7 @@
       <c r="D32" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="40"/>
+      <c r="E32" s="41"/>
       <c r="F32" s="8" t="s">
         <v>39</v>
       </c>
@@ -4521,7 +4521,7 @@
   <dimension ref="A1:Z38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4536,26 +4536,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
     </row>
     <row r="3" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -4621,7 +4621,7 @@
       <c r="D5" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="36" t="s">
         <v>55</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -4646,7 +4646,7 @@
       <c r="D6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="36"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="8" t="s">
         <v>38</v>
       </c>
@@ -4666,7 +4666,7 @@
       <c r="D7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="37"/>
+      <c r="E7" s="38"/>
       <c r="F7" s="8" t="s">
         <v>38</v>
       </c>
@@ -4686,7 +4686,7 @@
       <c r="D8" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="39" t="s">
         <v>47</v>
       </c>
       <c r="F8" s="15" t="s">
@@ -4710,7 +4710,7 @@
       <c r="D9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="39"/>
+      <c r="E9" s="40"/>
       <c r="F9" s="8" t="s">
         <v>39</v>
       </c>
@@ -4732,7 +4732,7 @@
       <c r="D10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="39"/>
+      <c r="E10" s="40"/>
       <c r="F10" s="8" t="s">
         <v>39</v>
       </c>
@@ -4754,7 +4754,7 @@
       <c r="D11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="40"/>
+      <c r="E11" s="41"/>
       <c r="F11" s="8" t="s">
         <v>39</v>
       </c>
@@ -4796,7 +4796,7 @@
       <c r="D13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="39" t="s">
         <v>47</v>
       </c>
       <c r="F13" s="8" t="s">
@@ -4818,7 +4818,7 @@
       <c r="D14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="39"/>
+      <c r="E14" s="40"/>
       <c r="F14" s="8" t="s">
         <v>38</v>
       </c>
@@ -4838,7 +4838,7 @@
       <c r="D15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="40"/>
+      <c r="E15" s="41"/>
       <c r="F15" s="8" t="s">
         <v>39</v>
       </c>
@@ -4882,7 +4882,7 @@
       <c r="D17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="39" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="8" t="s">
@@ -4906,7 +4906,7 @@
       <c r="D18" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E18" s="40"/>
+      <c r="E18" s="41"/>
       <c r="F18" s="8" t="s">
         <v>39</v>
       </c>
@@ -4928,7 +4928,7 @@
       <c r="D19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="39" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="8" t="s">
@@ -4950,7 +4950,7 @@
       <c r="D20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="39"/>
+      <c r="E20" s="40"/>
       <c r="F20" s="8" t="s">
         <v>38</v>
       </c>
@@ -4970,7 +4970,7 @@
       <c r="D21" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="39"/>
+      <c r="E21" s="40"/>
       <c r="F21" s="8" t="s">
         <v>38</v>
       </c>
@@ -4990,7 +4990,7 @@
       <c r="D22" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="39"/>
+      <c r="E22" s="40"/>
       <c r="F22" s="8" t="s">
         <v>38</v>
       </c>
@@ -5010,7 +5010,7 @@
       <c r="D23" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E23" s="39"/>
+      <c r="E23" s="40"/>
       <c r="F23" s="8" t="s">
         <v>38</v>
       </c>
@@ -5030,7 +5030,7 @@
       <c r="D24" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E24" s="40"/>
+      <c r="E24" s="41"/>
       <c r="F24" s="8" t="s">
         <v>38</v>
       </c>
@@ -5096,7 +5096,7 @@
       <c r="D27" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="39" t="s">
         <v>55</v>
       </c>
       <c r="F27" s="8" t="s">
@@ -5118,7 +5118,7 @@
       <c r="D28" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E28" s="39"/>
+      <c r="E28" s="40"/>
       <c r="F28" s="8" t="s">
         <v>38</v>
       </c>
@@ -5138,7 +5138,7 @@
       <c r="D29" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E29" s="39"/>
+      <c r="E29" s="40"/>
       <c r="F29" s="8" t="s">
         <v>38</v>
       </c>
@@ -5158,7 +5158,7 @@
       <c r="D30" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="40"/>
+      <c r="E30" s="41"/>
       <c r="F30" s="8" t="s">
         <v>38</v>
       </c>
@@ -5178,7 +5178,7 @@
       <c r="D31" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="38" t="s">
+      <c r="E31" s="39" t="s">
         <v>47</v>
       </c>
       <c r="F31" s="8" t="s">
@@ -5202,7 +5202,7 @@
       <c r="D32" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="40"/>
+      <c r="E32" s="41"/>
       <c r="F32" s="8" t="s">
         <v>39</v>
       </c>
@@ -5385,26 +5385,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
     </row>
     <row r="3" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -5468,7 +5468,7 @@
       <c r="D5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="36" t="s">
         <v>55</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -5493,7 +5493,7 @@
       <c r="D6" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E6" s="36"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="8" t="s">
         <v>38</v>
       </c>
@@ -5513,7 +5513,7 @@
       <c r="D7" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E7" s="36"/>
+      <c r="E7" s="37"/>
       <c r="F7" s="8" t="s">
         <v>38</v>
       </c>
@@ -5533,7 +5533,7 @@
       <c r="D8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="37"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="8" t="s">
         <v>38</v>
       </c>
@@ -5553,7 +5553,7 @@
       <c r="D9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="39" t="s">
         <v>47</v>
       </c>
       <c r="F9" s="8" t="s">
@@ -5577,7 +5577,7 @@
       <c r="D10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="39"/>
+      <c r="E10" s="40"/>
       <c r="F10" s="8" t="s">
         <v>39</v>
       </c>
@@ -5599,7 +5599,7 @@
       <c r="D11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="8" t="s">
         <v>39</v>
       </c>
@@ -5621,7 +5621,7 @@
       <c r="D12" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="8" t="s">
         <v>39</v>
       </c>
@@ -5643,7 +5643,7 @@
       <c r="D13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="39"/>
+      <c r="E13" s="40"/>
       <c r="F13" s="8" t="s">
         <v>39</v>
       </c>
@@ -5665,7 +5665,7 @@
       <c r="D14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="39"/>
+      <c r="E14" s="40"/>
       <c r="F14" s="8" t="s">
         <v>39</v>
       </c>
@@ -5687,7 +5687,7 @@
       <c r="D15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="39"/>
+      <c r="E15" s="40"/>
       <c r="F15" s="8" t="s">
         <v>39</v>
       </c>
@@ -5709,7 +5709,7 @@
       <c r="D16" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E16" s="39"/>
+      <c r="E16" s="40"/>
       <c r="F16" s="8" t="s">
         <v>39</v>
       </c>
@@ -5731,7 +5731,7 @@
       <c r="D17" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E17" s="39"/>
+      <c r="E17" s="40"/>
       <c r="F17" s="8" t="s">
         <v>39</v>
       </c>
@@ -5753,7 +5753,7 @@
       <c r="D18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="39"/>
+      <c r="E18" s="40"/>
       <c r="F18" s="8" t="s">
         <v>39</v>
       </c>
@@ -5775,7 +5775,7 @@
       <c r="D19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="39"/>
+      <c r="E19" s="40"/>
       <c r="F19" s="8" t="s">
         <v>39</v>
       </c>
@@ -5797,7 +5797,7 @@
       <c r="D20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="40"/>
+      <c r="E20" s="41"/>
       <c r="F20" s="8" t="s">
         <v>39</v>
       </c>
@@ -5819,7 +5819,7 @@
       <c r="D21" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="35" t="s">
+      <c r="E21" s="36" t="s">
         <v>55</v>
       </c>
       <c r="F21" s="8" t="s">
@@ -5841,7 +5841,7 @@
       <c r="D22" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="36"/>
+      <c r="E22" s="37"/>
       <c r="F22" s="15" t="s">
         <v>38</v>
       </c>
@@ -5861,7 +5861,7 @@
       <c r="D23" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="36"/>
+      <c r="E23" s="37"/>
       <c r="F23" s="8" t="s">
         <v>38</v>
       </c>
@@ -5881,7 +5881,7 @@
       <c r="D24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="37"/>
+      <c r="E24" s="38"/>
       <c r="F24" s="8" t="s">
         <v>38</v>
       </c>
@@ -5901,7 +5901,7 @@
       <c r="D25" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="38" t="s">
+      <c r="E25" s="39" t="s">
         <v>47</v>
       </c>
       <c r="F25" s="8" t="s">
@@ -5925,7 +5925,7 @@
       <c r="D26" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="39"/>
+      <c r="E26" s="40"/>
       <c r="F26" s="8" t="s">
         <v>39</v>
       </c>
@@ -5947,7 +5947,7 @@
       <c r="D27" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="39"/>
+      <c r="E27" s="40"/>
       <c r="F27" s="8" t="s">
         <v>39</v>
       </c>
@@ -5969,7 +5969,7 @@
       <c r="D28" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="39"/>
+      <c r="E28" s="40"/>
       <c r="F28" s="8" t="s">
         <v>39</v>
       </c>
@@ -5991,7 +5991,7 @@
       <c r="D29" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="40"/>
+      <c r="E29" s="41"/>
       <c r="F29" s="8" t="s">
         <v>39</v>
       </c>
@@ -6035,7 +6035,7 @@
       <c r="D31" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="38" t="s">
+      <c r="E31" s="39" t="s">
         <v>47</v>
       </c>
       <c r="F31" s="8" t="s">
@@ -6059,7 +6059,7 @@
       <c r="D32" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="39"/>
+      <c r="E32" s="40"/>
       <c r="F32" s="8" t="s">
         <v>39</v>
       </c>
@@ -6081,7 +6081,7 @@
       <c r="D33" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="39"/>
+      <c r="E33" s="40"/>
       <c r="F33" s="8" t="s">
         <v>39</v>
       </c>
@@ -6103,7 +6103,7 @@
       <c r="D34" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E34" s="40"/>
+      <c r="E34" s="41"/>
       <c r="F34" s="8" t="s">
         <v>39</v>
       </c>
@@ -6171,7 +6171,7 @@
       <c r="D37" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E37" s="38" t="s">
+      <c r="E37" s="39" t="s">
         <v>55</v>
       </c>
       <c r="F37" s="8" t="s">
@@ -6193,7 +6193,7 @@
       <c r="D38" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="40"/>
       <c r="F38" s="8" t="s">
         <v>38</v>
       </c>
@@ -6213,7 +6213,7 @@
       <c r="D39" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="40"/>
+      <c r="E39" s="41"/>
       <c r="F39" s="8" t="s">
         <v>38</v>
       </c>
@@ -6233,7 +6233,7 @@
       <c r="D40" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E40" s="38" t="s">
+      <c r="E40" s="39" t="s">
         <v>47</v>
       </c>
       <c r="F40" s="8" t="s">
@@ -6257,7 +6257,7 @@
       <c r="D41" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E41" s="39"/>
+      <c r="E41" s="40"/>
       <c r="F41" s="8" t="s">
         <v>39</v>
       </c>
@@ -6279,7 +6279,7 @@
       <c r="D42" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E42" s="39"/>
+      <c r="E42" s="40"/>
       <c r="F42" s="8" t="s">
         <v>39</v>
       </c>
@@ -6301,7 +6301,7 @@
       <c r="D43" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E43" s="39"/>
+      <c r="E43" s="40"/>
       <c r="F43" s="8" t="s">
         <v>39</v>
       </c>
@@ -6323,7 +6323,7 @@
       <c r="D44" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E44" s="39"/>
+      <c r="E44" s="40"/>
       <c r="F44" s="8" t="s">
         <v>39</v>
       </c>
@@ -6345,7 +6345,7 @@
       <c r="D45" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E45" s="39"/>
+      <c r="E45" s="40"/>
       <c r="F45" s="8" t="s">
         <v>39</v>
       </c>
@@ -6367,7 +6367,7 @@
       <c r="D46" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E46" s="39"/>
+      <c r="E46" s="40"/>
       <c r="F46" s="8" t="s">
         <v>39</v>
       </c>
@@ -6389,7 +6389,7 @@
       <c r="D47" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E47" s="39"/>
+      <c r="E47" s="40"/>
       <c r="F47" s="8" t="s">
         <v>39</v>
       </c>
@@ -6411,7 +6411,7 @@
       <c r="D48" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E48" s="39"/>
+      <c r="E48" s="40"/>
       <c r="F48" s="8" t="s">
         <v>39</v>
       </c>
@@ -6433,7 +6433,7 @@
       <c r="D49" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E49" s="39"/>
+      <c r="E49" s="40"/>
       <c r="F49" s="8" t="s">
         <v>39</v>
       </c>
@@ -6455,7 +6455,7 @@
       <c r="D50" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E50" s="40"/>
+      <c r="E50" s="41"/>
       <c r="F50" s="16" t="s">
         <v>39</v>
       </c>
@@ -6916,26 +6916,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>292</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
     </row>
     <row r="3" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -7048,7 +7048,7 @@
       <c r="D7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="39" t="s">
         <v>47</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -7072,7 +7072,7 @@
       <c r="D8" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="8" t="s">
         <v>39</v>
       </c>
@@ -7094,7 +7094,7 @@
       <c r="D9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="39"/>
+      <c r="E9" s="40"/>
       <c r="F9" s="8" t="s">
         <v>39</v>
       </c>
@@ -7116,7 +7116,7 @@
       <c r="D10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="39"/>
+      <c r="E10" s="40"/>
       <c r="F10" s="8" t="s">
         <v>39</v>
       </c>
@@ -7138,7 +7138,7 @@
       <c r="D11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="8" t="s">
         <v>39</v>
       </c>
@@ -7228,7 +7228,7 @@
       <c r="D15" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="36" t="s">
         <v>47</v>
       </c>
       <c r="F15" s="8" t="s">
@@ -7252,7 +7252,7 @@
       <c r="D16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="36"/>
+      <c r="E16" s="37"/>
       <c r="F16" s="8" t="s">
         <v>39</v>
       </c>
@@ -7274,7 +7274,7 @@
       <c r="D17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="36"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="8" t="s">
         <v>39</v>
       </c>
@@ -7296,7 +7296,7 @@
       <c r="D18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="36"/>
+      <c r="E18" s="37"/>
       <c r="F18" s="8" t="s">
         <v>39</v>
       </c>
@@ -7318,7 +7318,7 @@
       <c r="D19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="36"/>
+      <c r="E19" s="37"/>
       <c r="F19" s="8" t="s">
         <v>39</v>
       </c>
@@ -7340,7 +7340,7 @@
       <c r="D20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="36"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="8" t="s">
         <v>39</v>
       </c>
@@ -7362,7 +7362,7 @@
       <c r="D21" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="36"/>
+      <c r="E21" s="37"/>
       <c r="F21" s="8" t="s">
         <v>39</v>
       </c>
@@ -7384,7 +7384,7 @@
       <c r="D22" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="37"/>
+      <c r="E22" s="38"/>
       <c r="F22" s="8" t="s">
         <v>39</v>
       </c>
@@ -7428,7 +7428,7 @@
       <c r="D24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="35" t="s">
+      <c r="E24" s="36" t="s">
         <v>47</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -7452,7 +7452,7 @@
       <c r="D25" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="37"/>
+      <c r="E25" s="38"/>
       <c r="F25" s="8" t="s">
         <v>39</v>
       </c>
@@ -7474,7 +7474,7 @@
       <c r="D26" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="35" t="s">
+      <c r="E26" s="36" t="s">
         <v>55</v>
       </c>
       <c r="F26" s="8" t="s">
@@ -7496,7 +7496,7 @@
       <c r="D27" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E27" s="36"/>
+      <c r="E27" s="37"/>
       <c r="F27" s="8" t="s">
         <v>38</v>
       </c>
@@ -7516,7 +7516,7 @@
       <c r="D28" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="37"/>
+      <c r="E28" s="38"/>
       <c r="F28" s="8" t="s">
         <v>38</v>
       </c>
@@ -7536,7 +7536,7 @@
       <c r="D29" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="35" t="s">
+      <c r="E29" s="36" t="s">
         <v>47</v>
       </c>
       <c r="F29" s="8" t="s">
@@ -7560,7 +7560,7 @@
       <c r="D30" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="37"/>
+      <c r="E30" s="38"/>
       <c r="F30" s="18" t="s">
         <v>39</v>
       </c>
@@ -8021,8 +8021,8 @@
   </sheetPr>
   <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8037,26 +8037,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>405</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
     </row>
     <row r="3" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -8147,7 +8147,7 @@
       <c r="D6" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="42" t="s">
         <v>47</v>
       </c>
       <c r="F6" s="8" t="s">
@@ -8169,7 +8169,7 @@
       <c r="D7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="42"/>
+      <c r="E7" s="43"/>
       <c r="F7" s="8" t="s">
         <v>39</v>
       </c>
@@ -8191,7 +8191,7 @@
       <c r="D8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="43"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="8" t="s">
         <v>39</v>
       </c>
@@ -8928,8 +8928,8 @@
   </sheetPr>
   <dimension ref="A2:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8939,314 +8939,314 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="33" t="s">
         <v>387</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
     </row>
     <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
     </row>
     <row r="7" spans="2:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
     </row>
     <row r="8" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>1</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="48" t="s">
         <v>388</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
     </row>
     <row r="9" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>2</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="48" t="s">
         <v>389</v>
       </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
     </row>
     <row r="10" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>3</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="48" t="s">
         <v>390</v>
       </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
     </row>
     <row r="11" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>4</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="50" t="s">
         <v>391</v>
       </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
     </row>
     <row r="12" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>5</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="48" t="s">
         <v>397</v>
       </c>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
     </row>
     <row r="13" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>6</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="48" t="s">
         <v>392</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
     </row>
     <row r="14" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>7</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="48" t="s">
         <v>393</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
     </row>
     <row r="15" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>8</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="50" t="s">
         <v>394</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="45"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
     </row>
     <row r="16" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>9</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="48" t="s">
         <v>395</v>
       </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
     </row>
     <row r="17" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
         <v>10</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="48" t="s">
         <v>396</v>
       </c>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
-      <c r="B18" s="47">
+      <c r="B18" s="29">
         <v>11</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="45" t="s">
         <v>406</v>
       </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="50"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="47"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
-      <c r="B19" s="47">
+      <c r="B19" s="29">
         <v>12</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="45" t="s">
         <v>407</v>
       </c>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="50"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="47"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
-      <c r="B20" s="47">
+      <c r="B20" s="29">
         <v>13</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="45" t="s">
         <v>408</v>
       </c>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="50"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="47"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="28"/>
-      <c r="B21" s="47">
+      <c r="B21" s="29">
         <v>14</v>
       </c>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="45" t="s">
         <v>409</v>
       </c>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="50"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="47"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C14:K14"/>
+    <mergeCell ref="C15:K15"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="C13:K13"/>
+    <mergeCell ref="B2:K3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="C7:K7"/>
+    <mergeCell ref="C8:K8"/>
+    <mergeCell ref="C9:K9"/>
+    <mergeCell ref="C10:K10"/>
+    <mergeCell ref="C11:K11"/>
     <mergeCell ref="C18:K18"/>
     <mergeCell ref="C19:K19"/>
     <mergeCell ref="C20:K20"/>
     <mergeCell ref="C21:K21"/>
     <mergeCell ref="C16:K16"/>
     <mergeCell ref="C17:K17"/>
-    <mergeCell ref="C7:K7"/>
-    <mergeCell ref="C8:K8"/>
-    <mergeCell ref="C9:K9"/>
-    <mergeCell ref="C10:K10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="C13:K13"/>
-    <mergeCell ref="B2:K3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="C14:K14"/>
-    <mergeCell ref="C15:K15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" display="http://itcareer.pythonanywhere.com/"/>

</xml_diff>